<commit_message>
update it in 1031
</commit_message>
<xml_diff>
--- a/learn_chinese2021.xlsx
+++ b/learn_chinese2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="20210808" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="20210919" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="20211010" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="20211024" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="20211030" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="364">
   <si>
     <t xml:space="preserve">Chinese Lessons：</t>
   </si>
@@ -4729,9 +4730,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
     <t xml:space="preserve">shou zai de qu yu</t>
   </si>
   <si>
@@ -4877,6 +4875,731 @@
   </si>
   <si>
     <t xml:space="preserve">duì ā ，zán men xiàn zài jiù zuò 。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry-cleaned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 你要洗衣服吗？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Can I help you?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nǐ yào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">xǐ yī fú </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ma ？</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B: 是的，我想把这件衬衫干洗一下。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">B: Yes, i’d like this </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">shirt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to be dry-cleaned.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">shì de ，wǒ xiǎng bǎ zhè jiàn </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">chèn shān</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> gan xǐ yī xià 。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">T-shirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 好的，你想什么时候取衣服。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Sure, when do you want to get it back?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hǎo de ，nǐ xiǎng shen me shí hòu qǔ yī fú 。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B: 我下午要穿，你们这里能不能提供加急服务？</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">B:  I have to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006C3B"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">wear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> it this afternoon. Do you have an</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> urgent service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">wǒ xià wǔ yào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006C3B"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">chuān</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ，nǐ men zhè lǐ néng bú néng tí gòng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">jiā jí fú wù</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ？</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 有，但是要加收50%的费用，三个小时就洗好了。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">A: Yes, but we </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">charge</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 50% more and it only takes three hours.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">yǒu ，dàn shì yào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">jiā shōu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 50%de fèi yòng ，sān gè xiǎo shí jiù xǐ hǎo le </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">bai fen zhi 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B:好的，多少钱？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B: Okay. How much should I pay?&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hǎo de ，duō shǎo qián ？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 30美元。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Thirty dollars.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30měi yuán </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smoking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 亲爱的， 我觉得你要戒烟了。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">A: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006C3B"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Honey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, I think you should </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">quit smoking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006C3B"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">qīn ài de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ， wǒ jue dé nǐ yào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">jiè yān</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> le 。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B: 为什么？你以前不是说我抽烟的时候很性感吗？</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">B:  Why? You said I was </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">hot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> when smoking.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">wéi shen me ？nǐ yǐ qián bú shì shuō wǒ chōu yān de shí hòu hěn xìng gǎn ma ？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in the past time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 但是我更喜欢你健康。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: But I want you to be fit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dàn shì wǒ gèng xǐ huān nǐ jiàn kāng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B: 我知道吸烟有害健康。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">B: I know, Smoking is harmful to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">health</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">wǒ zhī dào xī yān yǒu hài </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">jiàn kāng</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 你看看这文章，上面说吸烟会导致肺癌。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">A: Check out this </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">article</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. It says smoking can lead to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006C3B"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">lung cancer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">nǐ kàn kàn zhè </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">wén zhāng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> ，shàng miàn shuō xī yān huì dǎo zhì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006C3B"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">fèi ái</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 。</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B: 我才不信呢。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B: I don’t believe it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wǒ cái bú xìn ne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: 别拐弯抹角了，你到底戒不戒烟</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">A: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Stop beating around the Bush</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. Will you quit or not?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">bié </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCE181E"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">guǎi wān mò jiǎo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> le ，nǐ dào dǐ jiè bú jiè yān </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">turn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">洗手</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xi shou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wash hands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">取钱</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qu qian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get my money back from bank.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">床</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chuang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ni bu shi shuo guo ai wo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same with </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ni shuo guo ai wo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hao kai xin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hao bu kai xin</t>
   </si>
 </sst>
 </file>
@@ -4886,7 +5609,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5088,18 +5811,6 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="等线"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="6.4"/>
-      <color rgb="FF4C4C4C"/>
-      <name val="Ubuntu"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5143,7 +5854,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5193,18 +5904,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6732,7 +7431,7 @@
   </sheetPr>
   <dimension ref="C2:AB34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -6780,7 +7479,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="4" t="s">
         <v>268</v>
       </c>
     </row>
@@ -6828,7 +7527,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="4" t="s">
         <v>278</v>
       </c>
     </row>
@@ -6875,65 +7574,402 @@
       <c r="U22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="15" t="s">
-        <v>286</v>
-      </c>
+      <c r="D23" s="11"/>
       <c r="F23" s="0"/>
       <c r="Q23" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D24" s="2"/>
       <c r="T24" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="T27" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="T30" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="T33" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="C2:AB56"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S46" activeCellId="0" sqref="S46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="1" width="2.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="2.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="2.64"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="1" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="U4" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="U7" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D11" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="U13" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="W14" s="0"/>
+      <c r="X14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="U16" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="W17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="7"/>
+      <c r="M18" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="U19" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="X20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="6"/>
+      <c r="X21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="U22" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D39" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="16.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F46" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="R51" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C52" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>